<commit_message>
english paper content update.
</commit_message>
<xml_diff>
--- a/document/模擬投資比較.xlsx
+++ b/document/模擬投資比較.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\StockPrediction\StockPrediction\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BE9854-D347-4339-B2F8-D3F5D37FD296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122C0948-9BE2-4615-BA06-ABBEE1FB47CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2745" yWindow="5865" windowWidth="10125" windowHeight="3300" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="模型成效比較 (2)" sheetId="12" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
   <si>
     <t>總損益</t>
   </si>
@@ -126,19 +126,42 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>準確率</t>
-  </si>
-  <si>
-    <t>精確率</t>
-  </si>
-  <si>
-    <t>召回率</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
     <t>RMSE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tradition-MLR</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tradition-ANN</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Window-ANN</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accuracy</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Precision</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recall</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Income</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Odds</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -147,10 +170,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="182" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="184" formatCode="0.0000_);[Red]\(0.0000\)"/>
-    <numFmt numFmtId="185" formatCode="0_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="178" formatCode="0.0000_);[Red]\(0.0000\)"/>
+    <numFmt numFmtId="179" formatCode="0_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -211,15 +234,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="185" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -228,6 +251,7 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -377,7 +401,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RMSE</c:v>
+                  <c:v>Income</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -399,13 +423,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>傳統法-MLR</c:v>
+                  <c:v>Tradition-MLR</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳統法-ANN</c:v>
+                  <c:v>Tradition-ANN</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>視窗法-ANN</c:v>
+                  <c:v>Window-ANN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -414,16 +438,16 @@
             <c:numRef>
               <c:f>'模型成效比較 (2)'!$B$2:$B$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10.2498</c:v>
+                  <c:v>0.76290000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.6379</c:v>
+                  <c:v>0.73809999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.1556999999999995</c:v>
+                  <c:v>0.92620000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -514,7 +538,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -795,7 +819,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>準確率</c:v>
+                  <c:v>Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -817,13 +841,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>傳統法-MLR</c:v>
+                  <c:v>Tradition-MLR</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳統法-ANN</c:v>
+                  <c:v>Tradition-ANN</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>視窗法-ANN</c:v>
+                  <c:v>Window-ANN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -861,7 +885,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>精確率</c:v>
+                  <c:v>Precision</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -883,13 +907,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>傳統法-MLR</c:v>
+                  <c:v>Tradition-MLR</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳統法-ANN</c:v>
+                  <c:v>Tradition-ANN</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>視窗法-ANN</c:v>
+                  <c:v>Window-ANN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -927,7 +951,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>召回率</c:v>
+                  <c:v>Recall</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -949,13 +973,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>傳統法-MLR</c:v>
+                  <c:v>Tradition-MLR</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳統法-ANN</c:v>
+                  <c:v>Tradition-ANN</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>視窗法-ANN</c:v>
+                  <c:v>Window-ANN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1017,13 +1041,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>傳統法-MLR</c:v>
+                  <c:v>Tradition-MLR</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳統法-ANN</c:v>
+                  <c:v>Tradition-ANN</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>視窗法-ANN</c:v>
+                  <c:v>Window-ANN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1413,7 +1437,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>準確率</c:v>
+                  <c:v>Accuracy</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2931,7 +2955,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>投資策略一</c:v>
+                  <c:v>Income</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2953,13 +2977,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>傳統法-MLR</c:v>
+                  <c:v>Tradition-MLR</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳統法-ANN</c:v>
+                  <c:v>Tradition-ANN</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>視窗法-ANN</c:v>
+                  <c:v>Window-ANN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2971,13 +2995,13 @@
                 <c:formatCode>0_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>114837</c:v>
+                  <c:v>191722</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-103851</c:v>
+                  <c:v>276595</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-339651</c:v>
+                  <c:v>325398</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2996,9 +3020,6 @@
               <c:f>總損益比較!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>投資策略二</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -3019,13 +3040,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>傳統法-MLR</c:v>
+                  <c:v>Tradition-MLR</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳統法-ANN</c:v>
+                  <c:v>Tradition-ANN</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>視窗法-ANN</c:v>
+                  <c:v>Window-ANN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3036,15 +3057,6 @@
               <c:numCache>
                 <c:formatCode>0_ </c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>88874</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>89873</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>44937</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3062,9 +3074,6 @@
               <c:f>總損益比較!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>投資策略三</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -3085,13 +3094,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>傳統法-MLR</c:v>
+                  <c:v>Tradition-MLR</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳統法-ANN</c:v>
+                  <c:v>Tradition-ANN</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>視窗法-ANN</c:v>
+                  <c:v>Window-ANN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3102,15 +3111,6 @@
               <c:numCache>
                 <c:formatCode>0_ </c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>191722</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>276595</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>325398</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3481,7 +3481,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>投資策略一</c:v>
+                  <c:v>Odds</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3503,13 +3503,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>傳統法-MLR</c:v>
+                  <c:v>Tradition-MLR</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳統法-ANN</c:v>
+                  <c:v>Tradition-ANN</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>視窗法-ANN</c:v>
+                  <c:v>Window-ANN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3521,13 +3521,13 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.66669999999999996</c:v>
+                  <c:v>0.76290000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26319999999999999</c:v>
+                  <c:v>0.73809999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20749999999999999</c:v>
+                  <c:v>0.92620000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3546,9 +3546,6 @@
               <c:f>勝率比較!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>投資策略二</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -3569,13 +3566,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>傳統法-MLR</c:v>
+                  <c:v>Tradition-MLR</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳統法-ANN</c:v>
+                  <c:v>Tradition-ANN</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>視窗法-ANN</c:v>
+                  <c:v>Window-ANN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3586,15 +3583,6 @@
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3612,9 +3600,6 @@
               <c:f>勝率比較!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>投資策略三</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -3635,13 +3620,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>傳統法-MLR</c:v>
+                  <c:v>Tradition-MLR</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>傳統法-ANN</c:v>
+                  <c:v>Tradition-ANN</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>視窗法-ANN</c:v>
+                  <c:v>Window-ANN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3652,15 +3637,6 @@
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.76290000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.73809999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.92620000000000002</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8176,8 +8152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD0B47B-2CEA-4A33-94FA-14FA8E388E68}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8190,7 +8166,7 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="5"/>
@@ -8198,10 +8174,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="13">
-        <v>10.2498</v>
+        <v>25</v>
+      </c>
+      <c r="B2" s="14">
+        <v>0.76290000000000002</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="12"/>
@@ -8210,10 +8186,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="13">
-        <v>11.6379</v>
+        <v>26</v>
+      </c>
+      <c r="B3" s="14">
+        <v>0.73809999999999998</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="12"/>
@@ -8226,10 +8202,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="13">
-        <v>9.1556999999999995</v>
+        <v>27</v>
+      </c>
+      <c r="B4" s="14">
+        <v>0.92620000000000002</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="12"/>
@@ -8269,7 +8245,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:C29"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8282,21 +8258,21 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B2" s="11">
         <v>0.70079999999999998</v>
@@ -8314,7 +8290,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B3" s="11">
         <v>0.68030000000000002</v>
@@ -8336,7 +8312,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B4" s="11">
         <v>0.75</v>
@@ -8362,7 +8338,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -8575,8 +8551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B58D985D-E2FD-490C-96B0-2DB8CFE8D32B}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8591,42 +8567,30 @@
         <v>8</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B2" s="7">
-        <v>114837</v>
-      </c>
-      <c r="C2" s="7">
-        <v>88874</v>
-      </c>
-      <c r="D2" s="7">
         <v>191722</v>
       </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B3" s="7">
-        <v>-103851</v>
-      </c>
-      <c r="C3" s="7">
-        <v>89873</v>
-      </c>
-      <c r="D3" s="7">
         <v>276595</v>
       </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -8635,17 +8599,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B4" s="7">
-        <v>-339651</v>
-      </c>
-      <c r="C4" s="7">
-        <v>44937</v>
-      </c>
-      <c r="D4" s="7">
         <v>325398</v>
       </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -8662,8 +8622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87588817-EF14-4320-B7D4-0CCF053C3204}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8674,46 +8634,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B2" s="10">
-        <v>0.66669999999999996</v>
-      </c>
-      <c r="C2" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="D2" s="10">
         <v>0.76290000000000002</v>
       </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B3" s="10">
-        <v>0.26319999999999999</v>
-      </c>
-      <c r="C3" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="D3" s="10">
         <v>0.73809999999999998</v>
       </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -8722,17 +8668,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B4" s="10">
-        <v>0.20749999999999999</v>
-      </c>
-      <c r="C4" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="10">
         <v>0.92620000000000002</v>
       </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>

</xml_diff>